<commit_message>
Fixing Assigning teacher to courses.
</commit_message>
<xml_diff>
--- a/CHARGES_enseignants_Février2017_2016-2017 (1).xlsx
+++ b/CHARGES_enseignants_Février2017_2016-2017 (1).xlsx
@@ -1,36 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="16925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amine\IdeaProjects\team-33\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adel\IdeaProjects\Team-33\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="833"/>
+    <workbookView tabRatio="833" windowHeight="7530" windowWidth="20490" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Charges-Février2017" sheetId="37" r:id="rId1"/>
+    <sheet name="Charges-Février2017" r:id="rId1" sheetId="37"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Charges-Février2017'!$A$1:$H$151</definedName>
-    <definedName name="a" localSheetId="0">#REF!</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'Charges-Février2017'!$A$1:$H$152</definedName>
+    <definedName localSheetId="0" name="a">#REF!</definedName>
     <definedName name="a">#REF!</definedName>
-    <definedName name="Charge" localSheetId="0">#REF!</definedName>
+    <definedName localSheetId="0" name="Charge">#REF!</definedName>
     <definedName name="Charge">#REF!</definedName>
-    <definedName name="Charges" localSheetId="0">'Charges-Février2017'!$A$1:$H$127</definedName>
+    <definedName localSheetId="0" name="Charges">'Charges-Février2017'!$A$1:$H$128</definedName>
     <definedName name="Charges">#REF!</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">'Charges-Février2017'!$1:$1</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Charges-Février2017'!$A$1:$H$127</definedName>
+    <definedName localSheetId="0" name="_xlnm.Print_Area">'Charges-Février2017'!$A$1:$H$128</definedName>
+    <definedName localSheetId="0" name="_xlnm.Print_Titles">'Charges-Février2017'!$1:$1</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="738" uniqueCount="524">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="784" uniqueCount="525">
   <si>
     <t>NOM</t>
   </si>
@@ -1686,11 +1686,15 @@
   <si>
     <t>D.Eddine</t>
   </si>
+  <si>
+    <t/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="0"/>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -1782,118 +1786,118 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="35">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="5" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="4" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="3" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="4" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="5" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyProtection="1" borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyProtection="1" borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="3" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="6" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" applyProtection="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyProtection="1" borderId="1" fillId="4" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="4" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyProtection="1" borderId="1" fillId="4" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="5" fontId="2" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" applyProtection="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="4" fontId="2" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyProtection="1" borderId="1" fillId="4" fontId="2" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1906,14 +1910,14 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -1948,7 +1952,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2000,7 +2004,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2105,7 +2109,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -2114,13 +2118,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -2130,7 +2134,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -2139,7 +2143,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -2148,7 +2152,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -2158,12 +2162,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -2194,7 +2198,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -2213,7 +2217,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -2225,30 +2229,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I127"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L127"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C118" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H128" sqref="A128:H133"/>
+    <sheetView tabSelected="1" workbookViewId="0" zoomScale="70" zoomScaleNormal="70">
+      <pane activePane="bottomRight" state="frozen" topLeftCell="C118" xSplit="2" ySplit="1"/>
+      <selection activeCell="C1" pane="topRight" sqref="C1"/>
+      <selection activeCell="A2" pane="bottomLeft" sqref="A2"/>
+      <selection activeCell="A128" pane="bottomRight" sqref="A128:XFD128"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.625" defaultRowHeight="11.25" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="11.25" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="19.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="30.125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.75" style="2" customWidth="1"/>
-    <col min="7" max="7" width="24" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="10.625" style="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="19.5" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="18.375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="2" width="12.625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="2" width="30.125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="2" width="24.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="2" width="29.75" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="2" width="24.0" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="2" width="13.625" collapsed="true"/>
+    <col min="9" max="16384" style="1" width="10.625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="42" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="42" r="1" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -2274,7 +2278,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="30" r="2" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A2" s="14" t="s">
         <v>301</v>
       </c>
@@ -2296,7 +2300,7 @@
       </c>
       <c r="H2" s="13"/>
     </row>
-    <row r="3" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="35.25" r="3" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A3" s="14" t="s">
         <v>303</v>
       </c>
@@ -2316,7 +2320,7 @@
       </c>
       <c r="H3" s="13"/>
     </row>
-    <row r="4" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="30" r="4" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A4" s="14" t="s">
         <v>305</v>
       </c>
@@ -2340,7 +2344,7 @@
       </c>
       <c r="H4" s="13"/>
     </row>
-    <row r="5" spans="1:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="40.5" r="5" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A5" s="14" t="s">
         <v>307</v>
       </c>
@@ -2364,7 +2368,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="35.25" r="6" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A6" s="14" t="s">
         <v>309</v>
       </c>
@@ -2388,7 +2392,7 @@
       </c>
       <c r="H6" s="15"/>
     </row>
-    <row r="7" spans="1:8" ht="42" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="42" r="7" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A7" s="14" t="s">
         <v>311</v>
       </c>
@@ -2408,7 +2412,7 @@
       <c r="G7" s="13"/>
       <c r="H7" s="15"/>
     </row>
-    <row r="8" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="30" r="8" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A8" s="14" t="s">
         <v>313</v>
       </c>
@@ -2428,7 +2432,7 @@
       <c r="G8" s="13"/>
       <c r="H8" s="13"/>
     </row>
-    <row r="9" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="30" r="9" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A9" s="14" t="s">
         <v>313</v>
       </c>
@@ -2452,7 +2456,7 @@
       </c>
       <c r="H9" s="13"/>
     </row>
-    <row r="10" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="30" r="10" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A10" s="14" t="s">
         <v>316</v>
       </c>
@@ -2474,7 +2478,7 @@
       <c r="G10" s="15"/>
       <c r="H10" s="13"/>
     </row>
-    <row r="11" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="30" r="11" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A11" s="14" t="s">
         <v>316</v>
       </c>
@@ -2494,7 +2498,7 @@
       <c r="G11" s="13"/>
       <c r="H11" s="13"/>
     </row>
-    <row r="12" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="30" r="12" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A12" s="14" t="s">
         <v>319</v>
       </c>
@@ -2518,7 +2522,7 @@
       </c>
       <c r="H12" s="8"/>
     </row>
-    <row r="13" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="30" r="13" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A13" s="14" t="s">
         <v>319</v>
       </c>
@@ -2542,7 +2546,7 @@
       </c>
       <c r="H13" s="16"/>
     </row>
-    <row r="14" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="30" r="14" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A14" s="25" t="s">
         <v>322</v>
       </c>
@@ -2560,7 +2564,7 @@
       <c r="G14" s="9"/>
       <c r="H14" s="23"/>
     </row>
-    <row r="15" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="30" r="15" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A15" s="14" t="s">
         <v>324</v>
       </c>
@@ -2582,7 +2586,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="30" r="16" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A16" s="14" t="s">
         <v>326</v>
       </c>
@@ -2606,7 +2610,7 @@
       </c>
       <c r="H16" s="13"/>
     </row>
-    <row r="17" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="30" r="17" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A17" s="14" t="s">
         <v>328</v>
       </c>
@@ -2628,7 +2632,7 @@
       <c r="G17" s="16"/>
       <c r="H17" s="13"/>
     </row>
-    <row r="18" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="30" r="18" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A18" s="14" t="s">
         <v>330</v>
       </c>
@@ -2652,7 +2656,7 @@
       </c>
       <c r="H18" s="13"/>
     </row>
-    <row r="19" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="37.5" r="19" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A19" s="14" t="s">
         <v>330</v>
       </c>
@@ -2672,7 +2676,7 @@
       </c>
       <c r="H19" s="16"/>
     </row>
-    <row r="20" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="30" r="20" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A20" s="14" t="s">
         <v>333</v>
       </c>
@@ -2694,7 +2698,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="36.75" r="21" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A21" s="14" t="s">
         <v>335</v>
       </c>
@@ -2716,7 +2720,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="30" r="22" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A22" s="14" t="s">
         <v>337</v>
       </c>
@@ -2738,7 +2742,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="30" r="23" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A23" s="14" t="s">
         <v>339</v>
       </c>
@@ -2758,7 +2762,7 @@
       <c r="G23" s="13"/>
       <c r="H23" s="13"/>
     </row>
-    <row r="24" spans="1:9" ht="44.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="44.25" r="24" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A24" s="14" t="s">
         <v>341</v>
       </c>
@@ -2780,7 +2784,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="30" r="25" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A25" s="14" t="s">
         <v>343</v>
       </c>
@@ -2800,7 +2804,7 @@
       </c>
       <c r="H25" s="13"/>
     </row>
-    <row r="26" spans="1:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="35.25" r="26" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A26" s="14" t="s">
         <v>345</v>
       </c>
@@ -2820,7 +2824,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="30" r="27" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A27" s="14" t="s">
         <v>347</v>
       </c>
@@ -2840,7 +2844,7 @@
       </c>
       <c r="H27" s="13"/>
     </row>
-    <row r="28" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="30" r="28" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A28" s="14" t="s">
         <v>349</v>
       </c>
@@ -2863,7 +2867,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="30" r="29" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A29" s="14" t="s">
         <v>350</v>
       </c>
@@ -2883,7 +2887,7 @@
       </c>
       <c r="H29" s="8"/>
     </row>
-    <row r="30" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="30" r="30" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A30" s="14" t="s">
         <v>352</v>
       </c>
@@ -2905,7 +2909,7 @@
       </c>
       <c r="H30" s="13"/>
     </row>
-    <row r="31" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="30" r="31" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A31" s="14" t="s">
         <v>353</v>
       </c>
@@ -2925,7 +2929,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="30" r="32" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A32" s="14" t="s">
         <v>355</v>
       </c>
@@ -2947,7 +2951,7 @@
       </c>
       <c r="H32" s="13"/>
     </row>
-    <row r="33" spans="1:8" ht="34.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="34.5" r="33" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A33" s="25" t="s">
         <v>356</v>
       </c>
@@ -2971,7 +2975,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="30" r="34" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A34" s="14" t="s">
         <v>357</v>
       </c>
@@ -2993,7 +2997,7 @@
       </c>
       <c r="H34" s="16"/>
     </row>
-    <row r="35" spans="1:8" ht="30" x14ac:dyDescent="0.15">
+    <row ht="30" r="35" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A35" s="14" t="s">
         <v>359</v>
       </c>
@@ -3017,7 +3021,7 @@
       </c>
       <c r="H35" s="13"/>
     </row>
-    <row r="36" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="30" r="36" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A36" s="14" t="s">
         <v>361</v>
       </c>
@@ -3039,7 +3043,7 @@
       </c>
       <c r="H36" s="13"/>
     </row>
-    <row r="37" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="30" r="37" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A37" s="14" t="s">
         <v>363</v>
       </c>
@@ -3059,7 +3063,7 @@
       </c>
       <c r="H37" s="16"/>
     </row>
-    <row r="38" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="30" r="38" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A38" s="14" t="s">
         <v>365</v>
       </c>
@@ -3081,7 +3085,7 @@
       </c>
       <c r="H38" s="13"/>
     </row>
-    <row r="39" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="30" r="39" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A39" s="14" t="s">
         <v>367</v>
       </c>
@@ -3105,7 +3109,7 @@
       </c>
       <c r="H39" s="13"/>
     </row>
-    <row r="40" spans="1:8" ht="36.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="36.75" r="40" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A40" s="14" t="s">
         <v>369</v>
       </c>
@@ -3129,7 +3133,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="40.5" r="41" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A41" s="14" t="s">
         <v>370</v>
       </c>
@@ -3149,7 +3153,7 @@
       </c>
       <c r="H41" s="13"/>
     </row>
-    <row r="42" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="30" r="42" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A42" s="14" t="s">
         <v>371</v>
       </c>
@@ -3169,7 +3173,7 @@
       <c r="G42" s="13"/>
       <c r="H42" s="13"/>
     </row>
-    <row r="43" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="30" r="43" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A43" s="14" t="s">
         <v>373</v>
       </c>
@@ -3191,7 +3195,7 @@
       </c>
       <c r="H43" s="16"/>
     </row>
-    <row r="44" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="30" r="44" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A44" s="25" t="s">
         <v>375</v>
       </c>
@@ -3211,7 +3215,7 @@
       </c>
       <c r="H44" s="13"/>
     </row>
-    <row r="45" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="30" r="45" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A45" s="14" t="s">
         <v>376</v>
       </c>
@@ -3231,7 +3235,7 @@
       <c r="G45" s="8"/>
       <c r="H45" s="13"/>
     </row>
-    <row r="46" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="30" r="46" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A46" s="14" t="s">
         <v>378</v>
       </c>
@@ -3253,7 +3257,7 @@
       </c>
       <c r="H46" s="13"/>
     </row>
-    <row r="47" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="30" r="47" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A47" s="25" t="s">
         <v>380</v>
       </c>
@@ -3275,7 +3279,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="30" r="48" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A48" s="14" t="s">
         <v>382</v>
       </c>
@@ -3299,7 +3303,7 @@
       </c>
       <c r="H48" s="13"/>
     </row>
-    <row r="49" spans="1:8" ht="37.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="37.5" r="49" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A49" s="14" t="s">
         <v>383</v>
       </c>
@@ -3319,7 +3323,7 @@
       </c>
       <c r="H49" s="13"/>
     </row>
-    <row r="50" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="30" r="50" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A50" s="14" t="s">
         <v>385</v>
       </c>
@@ -3339,7 +3343,7 @@
       </c>
       <c r="H50" s="13"/>
     </row>
-    <row r="51" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="30" r="51" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A51" s="25" t="s">
         <v>387</v>
       </c>
@@ -3363,7 +3367,7 @@
       </c>
       <c r="H51" s="13"/>
     </row>
-    <row r="52" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="30" r="52" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A52" s="25" t="s">
         <v>389</v>
       </c>
@@ -3385,7 +3389,7 @@
       </c>
       <c r="H52" s="13"/>
     </row>
-    <row r="53" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="30" r="53" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A53" s="14" t="s">
         <v>390</v>
       </c>
@@ -3407,7 +3411,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="54" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="30" r="54" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A54" s="14" t="s">
         <v>392</v>
       </c>
@@ -3431,7 +3435,7 @@
       </c>
       <c r="H54" s="16"/>
     </row>
-    <row r="55" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="30" r="55" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A55" s="14" t="s">
         <v>393</v>
       </c>
@@ -3455,7 +3459,7 @@
       </c>
       <c r="H55" s="13"/>
     </row>
-    <row r="56" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="30" r="56" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A56" s="14" t="s">
         <v>395</v>
       </c>
@@ -3481,7 +3485,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="57" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="30" r="57" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A57" s="14" t="s">
         <v>397</v>
       </c>
@@ -3503,7 +3507,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="58" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="30" r="58" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A58" s="14" t="s">
         <v>398</v>
       </c>
@@ -3523,7 +3527,7 @@
       <c r="G58" s="13"/>
       <c r="H58" s="13"/>
     </row>
-    <row r="59" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="30" r="59" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A59" s="14" t="s">
         <v>400</v>
       </c>
@@ -3545,7 +3549,7 @@
       </c>
       <c r="H59" s="13"/>
     </row>
-    <row r="60" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="30" r="60" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A60" s="14" t="s">
         <v>402</v>
       </c>
@@ -3569,7 +3573,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="61" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="30" r="61" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A61" s="14" t="s">
         <v>404</v>
       </c>
@@ -3593,7 +3597,7 @@
       </c>
       <c r="H61" s="13"/>
     </row>
-    <row r="62" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="30" r="62" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A62" s="14" t="s">
         <v>406</v>
       </c>
@@ -3613,7 +3617,7 @@
       </c>
       <c r="H62" s="8"/>
     </row>
-    <row r="63" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="30" r="63" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A63" s="14" t="s">
         <v>408</v>
       </c>
@@ -3635,7 +3639,7 @@
       </c>
       <c r="H63" s="8"/>
     </row>
-    <row r="64" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="30" r="64" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A64" s="14" t="s">
         <v>408</v>
       </c>
@@ -3659,7 +3663,7 @@
       </c>
       <c r="H64" s="13"/>
     </row>
-    <row r="65" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="30" r="65" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A65" s="14" t="s">
         <v>411</v>
       </c>
@@ -3679,7 +3683,7 @@
       </c>
       <c r="H65" s="13"/>
     </row>
-    <row r="66" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="30" r="66" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A66" s="14" t="s">
         <v>413</v>
       </c>
@@ -3699,7 +3703,7 @@
       </c>
       <c r="H66" s="13"/>
     </row>
-    <row r="67" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="30" r="67" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A67" s="14" t="s">
         <v>415</v>
       </c>
@@ -3723,7 +3727,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="68" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="30" r="68" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A68" s="14" t="s">
         <v>416</v>
       </c>
@@ -3745,7 +3749,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="69" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="30" r="69" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A69" s="14" t="s">
         <v>418</v>
       </c>
@@ -3765,7 +3769,7 @@
       <c r="G69" s="13"/>
       <c r="H69" s="13"/>
     </row>
-    <row r="70" spans="1:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="40.5" r="70" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A70" s="14" t="s">
         <v>420</v>
       </c>
@@ -3785,7 +3789,7 @@
       </c>
       <c r="H70" s="13"/>
     </row>
-    <row r="71" spans="1:8" ht="34.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="34.5" r="71" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A71" s="14" t="s">
         <v>422</v>
       </c>
@@ -3807,7 +3811,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="72" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="30" r="72" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A72" s="14" t="s">
         <v>424</v>
       </c>
@@ -3829,7 +3833,7 @@
       <c r="G72" s="18"/>
       <c r="H72" s="13"/>
     </row>
-    <row r="73" spans="1:8" ht="37.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="37.5" r="73" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A73" s="14" t="s">
         <v>426</v>
       </c>
@@ -3849,7 +3853,7 @@
       </c>
       <c r="H73" s="13"/>
     </row>
-    <row r="74" spans="1:8" ht="37.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="37.5" r="74" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A74" s="14" t="s">
         <v>428</v>
       </c>
@@ -3871,7 +3875,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="75" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="30" r="75" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A75" s="14" t="s">
         <v>430</v>
       </c>
@@ -3891,7 +3895,7 @@
       </c>
       <c r="H75" s="15"/>
     </row>
-    <row r="76" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="30" r="76" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A76" s="14" t="s">
         <v>432</v>
       </c>
@@ -3913,7 +3917,7 @@
       <c r="G76" s="16"/>
       <c r="H76" s="13"/>
     </row>
-    <row r="77" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="30" r="77" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A77" s="14" t="s">
         <v>434</v>
       </c>
@@ -3937,7 +3941,7 @@
       </c>
       <c r="H77" s="13"/>
     </row>
-    <row r="78" spans="1:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="53.25" r="78" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A78" s="14" t="s">
         <v>436</v>
       </c>
@@ -3961,7 +3965,7 @@
       </c>
       <c r="H78" s="15"/>
     </row>
-    <row r="79" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="30" r="79" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A79" s="14" t="s">
         <v>438</v>
       </c>
@@ -3981,7 +3985,7 @@
       <c r="G79" s="13"/>
       <c r="H79" s="13"/>
     </row>
-    <row r="80" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="30" r="80" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A80" s="14" t="s">
         <v>439</v>
       </c>
@@ -4001,7 +4005,7 @@
       </c>
       <c r="H80" s="13"/>
     </row>
-    <row r="81" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="30" r="81" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A81" s="14" t="s">
         <v>441</v>
       </c>
@@ -4023,7 +4027,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="82" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="35.25" r="82" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A82" s="14" t="s">
         <v>443</v>
       </c>
@@ -4043,7 +4047,7 @@
       </c>
       <c r="H82" s="16"/>
     </row>
-    <row r="83" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="30" r="83" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A83" s="14" t="s">
         <v>445</v>
       </c>
@@ -4065,7 +4069,7 @@
       </c>
       <c r="H83" s="13"/>
     </row>
-    <row r="84" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="30" r="84" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A84" s="14" t="s">
         <v>447</v>
       </c>
@@ -4089,7 +4093,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="85" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="30" r="85" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A85" s="14" t="s">
         <v>448</v>
       </c>
@@ -4111,7 +4115,7 @@
       </c>
       <c r="H85" s="13"/>
     </row>
-    <row r="86" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="39.75" r="86" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A86" s="14" t="s">
         <v>450</v>
       </c>
@@ -4135,7 +4139,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="87" spans="1:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="38.25" r="87" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A87" s="14" t="s">
         <v>451</v>
       </c>
@@ -4155,7 +4159,7 @@
       <c r="G87" s="13"/>
       <c r="H87" s="13"/>
     </row>
-    <row r="88" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="30" r="88" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A88" s="14" t="s">
         <v>453</v>
       </c>
@@ -4179,7 +4183,7 @@
       </c>
       <c r="H88" s="13"/>
     </row>
-    <row r="89" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="30" r="89" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A89" s="14" t="s">
         <v>455</v>
       </c>
@@ -4199,7 +4203,7 @@
       </c>
       <c r="H89" s="13"/>
     </row>
-    <row r="90" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="30" r="90" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A90" s="14" t="s">
         <v>457</v>
       </c>
@@ -4221,7 +4225,7 @@
       <c r="G90" s="13"/>
       <c r="H90" s="13"/>
     </row>
-    <row r="91" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="30" r="91" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A91" s="14" t="s">
         <v>459</v>
       </c>
@@ -4241,7 +4245,7 @@
       </c>
       <c r="H91" s="13"/>
     </row>
-    <row r="92" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="30" r="92" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A92" s="14" t="s">
         <v>461</v>
       </c>
@@ -4263,7 +4267,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="93" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="30" r="93" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A93" s="14" t="s">
         <v>462</v>
       </c>
@@ -4283,7 +4287,7 @@
       <c r="G93" s="13"/>
       <c r="H93" s="13"/>
     </row>
-    <row r="94" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="30" r="94" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A94" s="14" t="s">
         <v>464</v>
       </c>
@@ -4301,7 +4305,7 @@
       <c r="G94" s="23"/>
       <c r="H94" s="23"/>
     </row>
-    <row r="95" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="30" r="95" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A95" s="14" t="s">
         <v>465</v>
       </c>
@@ -4323,7 +4327,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="96" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="30" r="96" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A96" s="14" t="s">
         <v>467</v>
       </c>
@@ -4345,7 +4349,7 @@
       </c>
       <c r="H96" s="13"/>
     </row>
-    <row r="97" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="30" r="97" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A97" s="14" t="s">
         <v>469</v>
       </c>
@@ -4367,7 +4371,7 @@
       </c>
       <c r="H97" s="13"/>
     </row>
-    <row r="98" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="30" r="98" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A98" s="14" t="s">
         <v>470</v>
       </c>
@@ -4387,7 +4391,7 @@
       </c>
       <c r="H98" s="13"/>
     </row>
-    <row r="99" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="30" r="99" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A99" s="14" t="s">
         <v>471</v>
       </c>
@@ -4407,7 +4411,7 @@
       </c>
       <c r="H99" s="13"/>
     </row>
-    <row r="100" spans="1:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="40.5" r="100" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A100" s="14" t="s">
         <v>473</v>
       </c>
@@ -4429,7 +4433,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="101" spans="1:8" ht="36.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="36.75" r="101" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A101" s="14" t="s">
         <v>475</v>
       </c>
@@ -4453,7 +4457,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="102" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="30" r="102" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A102" s="14" t="s">
         <v>477</v>
       </c>
@@ -4475,7 +4479,7 @@
       <c r="G102" s="13"/>
       <c r="H102" s="15"/>
     </row>
-    <row r="103" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="30" r="103" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A103" s="14" t="s">
         <v>479</v>
       </c>
@@ -4495,7 +4499,7 @@
       </c>
       <c r="H103" s="13"/>
     </row>
-    <row r="104" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="30" r="104" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A104" s="14" t="s">
         <v>481</v>
       </c>
@@ -4515,7 +4519,7 @@
       </c>
       <c r="H104" s="13"/>
     </row>
-    <row r="105" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="30" r="105" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A105" s="14" t="s">
         <v>483</v>
       </c>
@@ -4537,7 +4541,7 @@
       </c>
       <c r="H105" s="13"/>
     </row>
-    <row r="106" spans="1:8" ht="36.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="36.75" r="106" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A106" s="14" t="s">
         <v>484</v>
       </c>
@@ -4559,7 +4563,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="107" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="30" r="107" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A107" s="14" t="s">
         <v>486</v>
       </c>
@@ -4583,7 +4587,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="108" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="30" r="108" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A108" s="14" t="s">
         <v>488</v>
       </c>
@@ -4605,7 +4609,7 @@
       </c>
       <c r="H108" s="13"/>
     </row>
-    <row r="109" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="30" r="109" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A109" s="14" t="s">
         <v>490</v>
       </c>
@@ -4627,7 +4631,7 @@
       </c>
       <c r="H109" s="13"/>
     </row>
-    <row r="110" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="30" r="110" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A110" s="25" t="s">
         <v>492</v>
       </c>
@@ -4649,7 +4653,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="111" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="30" r="111" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A111" s="14" t="s">
         <v>494</v>
       </c>
@@ -4671,7 +4675,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="112" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="30" r="112" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A112" s="14" t="s">
         <v>496</v>
       </c>
@@ -4693,7 +4697,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="113" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="30" r="113" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A113" s="14" t="s">
         <v>498</v>
       </c>
@@ -4715,7 +4719,7 @@
       <c r="G113" s="15"/>
       <c r="H113" s="13"/>
     </row>
-    <row r="114" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="30" r="114" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A114" s="14" t="s">
         <v>500</v>
       </c>
@@ -4735,7 +4739,7 @@
       <c r="G114" s="13"/>
       <c r="H114" s="15"/>
     </row>
-    <row r="115" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="30" r="115" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A115" s="14" t="s">
         <v>501</v>
       </c>
@@ -4757,7 +4761,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="116" spans="1:9" ht="57" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="57" r="116" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A116" s="14" t="s">
         <v>502</v>
       </c>
@@ -4777,7 +4781,7 @@
       </c>
       <c r="H116" s="15"/>
     </row>
-    <row r="117" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="30" r="117" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A117" s="14" t="s">
         <v>503</v>
       </c>
@@ -4799,7 +4803,7 @@
       </c>
       <c r="H117" s="13"/>
     </row>
-    <row r="118" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="30" r="118" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A118" s="14" t="s">
         <v>505</v>
       </c>
@@ -4819,196 +4823,286 @@
       </c>
       <c r="H118" s="13"/>
     </row>
-    <row r="119" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row customHeight="1" ht="30" r="119" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A119" s="14" t="s">
-        <v>507</v>
+        <v>509</v>
       </c>
       <c r="B119" s="14" t="s">
-        <v>508</v>
-      </c>
-      <c r="C119" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="D119" s="16"/>
+        <v>510</v>
+      </c>
+      <c r="C119" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="D119" s="13" t="s">
+        <v>524</v>
+      </c>
       <c r="E119" s="13" t="s">
-        <v>206</v>
-      </c>
-      <c r="F119" s="13"/>
+        <v>195</v>
+      </c>
+      <c r="F119" s="8" t="s">
+        <v>108</v>
+      </c>
       <c r="G119" s="13" t="s">
-        <v>227</v>
-      </c>
-      <c r="H119" s="13"/>
-    </row>
-    <row r="120" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+        <v>262</v>
+      </c>
+      <c r="H119" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="I119"/>
+    </row>
+    <row customHeight="1" ht="30" r="120" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A120" s="14" t="s">
-        <v>509</v>
+        <v>511</v>
       </c>
       <c r="B120" s="14" t="s">
-        <v>510</v>
-      </c>
-      <c r="C120" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="D120" s="13"/>
+        <v>401</v>
+      </c>
+      <c r="C120" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D120" s="13" t="s">
+        <v>524</v>
+      </c>
       <c r="E120" s="13" t="s">
-        <v>195</v>
-      </c>
-      <c r="F120" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="G120" s="13" t="s">
-        <v>262</v>
+        <v>17</v>
+      </c>
+      <c r="F120" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="G120" s="8" t="s">
+        <v>107</v>
       </c>
       <c r="H120" s="15" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="121" spans="1:9" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I120"/>
+    </row>
+    <row customHeight="1" ht="39.75" r="121" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A121" s="14" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="B121" s="14" t="s">
-        <v>401</v>
-      </c>
-      <c r="C121" s="12" t="s">
+        <v>513</v>
+      </c>
+      <c r="C121" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D121" s="13" t="s">
+        <v>524</v>
+      </c>
+      <c r="E121" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="F121" s="13" t="s">
+        <v>524</v>
+      </c>
+      <c r="G121" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="H121" s="13" t="s">
+        <v>524</v>
+      </c>
+      <c r="I121"/>
+    </row>
+    <row customHeight="1" ht="30" r="122" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A122" s="14" t="s">
+        <v>514</v>
+      </c>
+      <c r="B122" s="14" t="s">
+        <v>515</v>
+      </c>
+      <c r="C122" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D121" s="13"/>
-      <c r="E121" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="F121" s="13" t="s">
-        <v>106</v>
-      </c>
-      <c r="G121" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="H121" s="15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="122" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A122" s="14" t="s">
-        <v>512</v>
-      </c>
-      <c r="B122" s="14" t="s">
-        <v>513</v>
-      </c>
-      <c r="C122" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="D122" s="13"/>
+      <c r="D122" s="8" t="s">
+        <v>56</v>
+      </c>
       <c r="E122" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="F122" s="13"/>
+        <v>524</v>
+      </c>
+      <c r="F122" s="8" t="s">
+        <v>54</v>
+      </c>
       <c r="G122" s="13" t="s">
-        <v>112</v>
-      </c>
-      <c r="H122" s="13"/>
-    </row>
-    <row r="123" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A123" s="14" t="s">
-        <v>514</v>
-      </c>
-      <c r="B123" s="14" t="s">
-        <v>515</v>
-      </c>
-      <c r="C123" s="12" t="s">
+        <v>524</v>
+      </c>
+      <c r="H122" s="13" t="s">
+        <v>524</v>
+      </c>
+      <c r="I122"/>
+    </row>
+    <row customHeight="1" ht="37.5" r="123" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A123" s="29" t="s">
+        <v>516</v>
+      </c>
+      <c r="B123" s="29" t="s">
+        <v>517</v>
+      </c>
+      <c r="C123" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="D123" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="E123" s="13"/>
-      <c r="F123" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="G123" s="13"/>
-      <c r="H123" s="13"/>
-    </row>
-    <row r="124" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D123" s="23" t="s">
+        <v>524</v>
+      </c>
+      <c r="E123" s="23" t="s">
+        <v>524</v>
+      </c>
+      <c r="F123" s="23" t="s">
+        <v>524</v>
+      </c>
+      <c r="G123" s="30" t="s">
+        <v>524</v>
+      </c>
+      <c r="H123" s="22" t="s">
+        <v>524</v>
+      </c>
+      <c r="I123" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="J123" t="s">
+        <v>524</v>
+      </c>
+      <c r="K123"/>
+    </row>
+    <row customHeight="1" ht="30" r="124" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A124" s="29" t="s">
-        <v>516</v>
+        <v>518</v>
       </c>
       <c r="B124" s="29" t="s">
-        <v>517</v>
+        <v>519</v>
       </c>
       <c r="C124" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="D124" s="23"/>
-      <c r="E124" s="23"/>
-      <c r="F124" s="23"/>
-      <c r="G124" s="30"/>
-      <c r="H124" s="22"/>
+      <c r="D124" s="23" t="s">
+        <v>524</v>
+      </c>
+      <c r="E124" s="23" t="s">
+        <v>524</v>
+      </c>
+      <c r="F124" s="23" t="s">
+        <v>524</v>
+      </c>
+      <c r="G124" s="23" t="s">
+        <v>524</v>
+      </c>
+      <c r="H124" s="22" t="s">
+        <v>524</v>
+      </c>
       <c r="I124" s="1" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="125" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A125" s="29" t="s">
-        <v>518</v>
-      </c>
-      <c r="B125" s="29" t="s">
-        <v>519</v>
-      </c>
-      <c r="C125" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="D125" s="23"/>
-      <c r="E125" s="23"/>
-      <c r="F125" s="23"/>
-      <c r="G125" s="23"/>
-      <c r="H125" s="22"/>
+      <c r="J124" t="s">
+        <v>524</v>
+      </c>
+      <c r="K124"/>
+    </row>
+    <row customHeight="1" ht="30" r="125" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A125" s="31" t="s">
+        <v>520</v>
+      </c>
+      <c r="B125" s="31" t="s">
+        <v>521</v>
+      </c>
+      <c r="C125" s="24" t="s">
+        <v>524</v>
+      </c>
+      <c r="D125" s="24" t="s">
+        <v>524</v>
+      </c>
+      <c r="E125" s="5" t="s">
+        <v>524</v>
+      </c>
+      <c r="F125" s="23" t="s">
+        <v>524</v>
+      </c>
+      <c r="G125" s="5" t="s">
+        <v>524</v>
+      </c>
+      <c r="H125" s="23" t="s">
+        <v>524</v>
+      </c>
       <c r="I125" s="1" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="126" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="J125" t="s">
+        <v>524</v>
+      </c>
+      <c r="K125"/>
+    </row>
+    <row customHeight="1" ht="30" r="126" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A126" s="31" t="s">
-        <v>520</v>
+        <v>522</v>
       </c>
       <c r="B126" s="31" t="s">
-        <v>521</v>
-      </c>
-      <c r="C126" s="24"/>
-      <c r="D126" s="24"/>
-      <c r="E126" s="5"/>
-      <c r="F126" s="23"/>
-      <c r="G126" s="5"/>
-      <c r="H126" s="23"/>
+        <v>523</v>
+      </c>
+      <c r="C126" s="24" t="s">
+        <v>524</v>
+      </c>
+      <c r="D126" s="23" t="s">
+        <v>524</v>
+      </c>
+      <c r="E126" s="24" t="s">
+        <v>524</v>
+      </c>
+      <c r="F126" s="23" t="s">
+        <v>524</v>
+      </c>
+      <c r="G126" s="23" t="s">
+        <v>524</v>
+      </c>
+      <c r="H126" s="23" t="s">
+        <v>524</v>
+      </c>
       <c r="I126" s="1" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="127" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A127" s="31" t="s">
-        <v>522</v>
-      </c>
-      <c r="B127" s="31" t="s">
-        <v>523</v>
-      </c>
-      <c r="C127" s="24"/>
-      <c r="D127" s="23"/>
-      <c r="E127" s="24"/>
-      <c r="F127" s="23"/>
-      <c r="G127" s="23"/>
-      <c r="H127" s="23"/>
-      <c r="I127" s="1" t="s">
-        <v>300</v>
-      </c>
+      <c r="J126" t="s">
+        <v>524</v>
+      </c>
+      <c r="K126"/>
+    </row>
+    <row customHeight="1" ht="30" r="127" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A127" s="14" t="s">
+        <v>507</v>
+      </c>
+      <c r="B127" s="14" t="s">
+        <v>508</v>
+      </c>
+      <c r="C127" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="D127" s="16" t="s">
+        <v>524</v>
+      </c>
+      <c r="E127" s="13" t="s">
+        <v>206</v>
+      </c>
+      <c r="F127" s="13" t="s">
+        <v>524</v>
+      </c>
+      <c r="G127" s="13" t="s">
+        <v>227</v>
+      </c>
+      <c r="H127" s="13" t="s">
+        <v>524</v>
+      </c>
+      <c r="I127" t="s">
+        <v>524</v>
+      </c>
+      <c r="J127"/>
     </row>
   </sheetData>
   <sortState ref="A127:Q133">
     <sortCondition ref="A127"/>
   </sortState>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
-  <pageMargins left="1.1023622047244095" right="1.1417322834645669" top="0.51181102362204722" bottom="0.98425196850393704" header="0.51181102362204722" footer="0.51181102362204722"/>
-  <pageSetup paperSize="9" scale="67" orientation="landscape" r:id="rId1"/>
+  <pageMargins bottom="0.98425196850393704" footer="0.51181102362204722" header="0.51181102362204722" left="1.1023622047244095" right="1.1417322834645669" top="0.51181102362204722"/>
+  <pageSetup orientation="landscape" paperSize="9" r:id="rId1" scale="67"/>
   <headerFooter alignWithMargins="0"/>
   <rowBreaks count="1" manualBreakCount="1">
-    <brk id="33" max="14" man="1"/>
+    <brk id="33" man="1" max="14"/>
   </rowBreaks>
 </worksheet>
 </file>
</xml_diff>